<commit_message>
import covid-19 vaccionation objects list from excel file successfully
</commit_message>
<xml_diff>
--- a/Resource/import.xlsx
+++ b/Resource/import.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AN$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AN$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="349">
   <si>
     <t>STT</t>
   </si>
@@ -1063,6 +1063,9 @@
   </si>
   <si>
     <t>741 Tạ Quang Bưu</t>
+  </si>
+  <si>
+    <t>Trung tâm y tế huyện Chư Sê</t>
   </si>
 </sst>
 </file>
@@ -1495,32 +1498,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="G88" workbookViewId="0">
+      <selection activeCell="M1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1612,8 +1615,8 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>64007</v>
+      <c r="B2" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>19</v>
@@ -1650,8 +1653,8 @@
       <c r="O2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="11">
-        <v>64007</v>
+      <c r="P2" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>27</v>
@@ -1662,8 +1665,8 @@
       <c r="S2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="11">
-        <v>64007</v>
+      <c r="T2" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U2" s="9"/>
       <c r="V2" s="12"/>
@@ -1691,8 +1694,8 @@
         <f t="shared" ref="A3:A66" si="0" xml:space="preserve"> A2 + 1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="7">
-        <v>64007</v>
+      <c r="B3" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>31</v>
@@ -1729,8 +1732,8 @@
       <c r="O3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="11">
-        <v>64007</v>
+      <c r="P3" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q3" s="9" t="s">
         <v>36</v>
@@ -1741,8 +1744,8 @@
       <c r="S3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="11">
-        <v>64007</v>
+      <c r="T3" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U3" s="9"/>
       <c r="V3" s="12"/>
@@ -1770,8 +1773,8 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="7">
-        <v>64007</v>
+      <c r="B4" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>31</v>
@@ -1808,8 +1811,8 @@
       <c r="O4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="11">
-        <v>64007</v>
+      <c r="P4" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>36</v>
@@ -1820,8 +1823,8 @@
       <c r="S4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="11">
-        <v>64007</v>
+      <c r="T4" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="12"/>
@@ -1849,8 +1852,8 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="7">
-        <v>64007</v>
+      <c r="B5" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>41</v>
@@ -1887,8 +1890,8 @@
       <c r="O5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P5" s="11">
-        <v>64007</v>
+      <c r="P5" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q5" s="9" t="s">
         <v>27</v>
@@ -1899,8 +1902,8 @@
       <c r="S5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="11">
-        <v>64007</v>
+      <c r="T5" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="12"/>
@@ -1928,8 +1931,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>64007</v>
+      <c r="B6" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>52</v>
@@ -1966,8 +1969,8 @@
       <c r="O6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P6" s="11">
-        <v>64007</v>
+      <c r="P6" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q6" s="9" t="s">
         <v>36</v>
@@ -1978,8 +1981,8 @@
       <c r="S6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="11">
-        <v>64007</v>
+      <c r="T6" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U6" s="9"/>
       <c r="V6" s="12"/>
@@ -2007,8 +2010,8 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="7">
-        <v>64007</v>
+      <c r="B7" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>57</v>
@@ -2047,8 +2050,8 @@
       <c r="O7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="11">
-        <v>64007</v>
+      <c r="P7" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>62</v>
@@ -2059,8 +2062,8 @@
       <c r="S7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="T7" s="11">
-        <v>64007</v>
+      <c r="T7" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U7" s="9"/>
       <c r="V7" s="12"/>
@@ -2088,8 +2091,8 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="7">
-        <v>64007</v>
+      <c r="B8" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>66</v>
@@ -2128,8 +2131,8 @@
       <c r="O8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="P8" s="11">
-        <v>64007</v>
+      <c r="P8" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q8" s="9" t="s">
         <v>62</v>
@@ -2140,8 +2143,8 @@
       <c r="S8" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="T8" s="11">
-        <v>64007</v>
+      <c r="T8" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U8" s="9"/>
       <c r="V8" s="12"/>
@@ -2169,8 +2172,8 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="7">
-        <v>64007</v>
+      <c r="B9" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>74</v>
@@ -2209,8 +2212,8 @@
       <c r="O9" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="P9" s="11">
-        <v>64007</v>
+      <c r="P9" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>62</v>
@@ -2221,8 +2224,8 @@
       <c r="S9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="T9" s="11">
-        <v>64007</v>
+      <c r="T9" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U9" s="9"/>
       <c r="V9" s="12"/>
@@ -2250,8 +2253,8 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="7">
-        <v>64007</v>
+      <c r="B10" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>80</v>
@@ -2290,8 +2293,8 @@
       <c r="O10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="11">
-        <v>64007</v>
+      <c r="P10" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q10" s="9" t="s">
         <v>62</v>
@@ -2302,8 +2305,8 @@
       <c r="S10" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="T10" s="11">
-        <v>64007</v>
+      <c r="T10" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U10" s="9"/>
       <c r="V10" s="12"/>
@@ -2331,8 +2334,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="7">
-        <v>64007</v>
+      <c r="B11" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>84</v>
@@ -2371,8 +2374,8 @@
       <c r="O11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="P11" s="11">
-        <v>64007</v>
+      <c r="P11" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>62</v>
@@ -2383,8 +2386,8 @@
       <c r="S11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="T11" s="11">
-        <v>64007</v>
+      <c r="T11" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U11" s="9"/>
       <c r="V11" s="12"/>
@@ -2412,8 +2415,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="7">
-        <v>64007</v>
+      <c r="B12" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>88</v>
@@ -2450,8 +2453,8 @@
       <c r="O12" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="P12" s="11">
-        <v>64007</v>
+      <c r="P12" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q12" s="9" t="s">
         <v>36</v>
@@ -2462,8 +2465,8 @@
       <c r="S12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T12" s="11">
-        <v>64007</v>
+      <c r="T12" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U12" s="9"/>
       <c r="V12" s="12"/>
@@ -2491,8 +2494,8 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="7">
-        <v>64007</v>
+      <c r="B13" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>95</v>
@@ -2531,8 +2534,8 @@
       <c r="O13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="P13" s="11">
-        <v>64007</v>
+      <c r="P13" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q13" s="9" t="s">
         <v>36</v>
@@ -2543,8 +2546,8 @@
       <c r="S13" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="T13" s="11">
-        <v>64007</v>
+      <c r="T13" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U13" s="9"/>
       <c r="V13" s="12"/>
@@ -2572,8 +2575,8 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="7">
-        <v>64007</v>
+      <c r="B14" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>103</v>
@@ -2612,8 +2615,8 @@
       <c r="O14" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="P14" s="11">
-        <v>64007</v>
+      <c r="P14" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>36</v>
@@ -2624,8 +2627,8 @@
       <c r="S14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="T14" s="11">
-        <v>64007</v>
+      <c r="T14" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U14" s="9"/>
       <c r="V14" s="12"/>
@@ -2653,8 +2656,8 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="7">
-        <v>64007</v>
+      <c r="B15" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>108</v>
@@ -2691,8 +2694,8 @@
         <v>114</v>
       </c>
       <c r="O15" s="9"/>
-      <c r="P15" s="11">
-        <v>64007</v>
+      <c r="P15" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q15" s="9"/>
       <c r="R15" s="10"/>
@@ -2724,8 +2727,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="7">
-        <v>64007</v>
+      <c r="B16" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>115</v>
@@ -2762,8 +2765,8 @@
       <c r="O16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P16" s="11">
-        <v>64007</v>
+      <c r="P16" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q16" s="9" t="s">
         <v>36</v>
@@ -2774,8 +2777,8 @@
       <c r="S16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="T16" s="11">
-        <v>64007</v>
+      <c r="T16" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U16" s="9"/>
       <c r="V16" s="12"/>
@@ -2803,8 +2806,8 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="7">
-        <v>64007</v>
+      <c r="B17" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>121</v>
@@ -2841,8 +2844,8 @@
       <c r="O17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P17" s="11">
-        <v>64007</v>
+      <c r="P17" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q17" s="9" t="s">
         <v>27</v>
@@ -2853,8 +2856,8 @@
       <c r="S17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T17" s="11">
-        <v>64007</v>
+      <c r="T17" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U17" s="9"/>
       <c r="V17" s="12"/>
@@ -2882,8 +2885,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="7">
-        <v>64007</v>
+      <c r="B18" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>121</v>
@@ -2920,8 +2923,8 @@
       <c r="O18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="11">
-        <v>64007</v>
+      <c r="P18" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q18" s="9" t="s">
         <v>27</v>
@@ -2932,8 +2935,8 @@
       <c r="S18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T18" s="11">
-        <v>64007</v>
+      <c r="T18" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U18" s="9"/>
       <c r="V18" s="12"/>
@@ -2961,8 +2964,8 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="7">
-        <v>64007</v>
+      <c r="B19" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>126</v>
@@ -2999,8 +3002,8 @@
       <c r="O19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P19" s="11">
-        <v>64007</v>
+      <c r="P19" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q19" s="9" t="s">
         <v>27</v>
@@ -3011,8 +3014,8 @@
       <c r="S19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T19" s="11">
-        <v>64007</v>
+      <c r="T19" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U19" s="9"/>
       <c r="V19" s="12"/>
@@ -3040,8 +3043,8 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="7">
-        <v>64007</v>
+      <c r="B20" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>126</v>
@@ -3078,8 +3081,8 @@
       <c r="O20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P20" s="11">
-        <v>64007</v>
+      <c r="P20" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q20" s="9" t="s">
         <v>27</v>
@@ -3090,8 +3093,8 @@
       <c r="S20" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T20" s="11">
-        <v>64007</v>
+      <c r="T20" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U20" s="9"/>
       <c r="V20" s="12"/>
@@ -3119,8 +3122,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="7">
-        <v>64007</v>
+      <c r="B21" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>130</v>
@@ -3157,8 +3160,8 @@
       <c r="O21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="11">
-        <v>64007</v>
+      <c r="P21" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q21" s="9" t="s">
         <v>27</v>
@@ -3169,8 +3172,8 @@
       <c r="S21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T21" s="11">
-        <v>64007</v>
+      <c r="T21" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U21" s="9"/>
       <c r="V21" s="12"/>
@@ -3198,8 +3201,8 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="7">
-        <v>64007</v>
+      <c r="B22" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>130</v>
@@ -3236,8 +3239,8 @@
       <c r="O22" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P22" s="11">
-        <v>64007</v>
+      <c r="P22" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q22" s="9" t="s">
         <v>27</v>
@@ -3248,8 +3251,8 @@
       <c r="S22" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T22" s="11">
-        <v>64007</v>
+      <c r="T22" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U22" s="9"/>
       <c r="V22" s="12"/>
@@ -3277,8 +3280,8 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="7">
-        <v>64007</v>
+      <c r="B23" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>134</v>
@@ -3315,8 +3318,8 @@
       <c r="O23" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P23" s="11">
-        <v>64007</v>
+      <c r="P23" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q23" s="9" t="s">
         <v>27</v>
@@ -3327,8 +3330,8 @@
       <c r="S23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T23" s="11">
-        <v>64007</v>
+      <c r="T23" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U23" s="9"/>
       <c r="V23" s="12"/>
@@ -3356,8 +3359,8 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="7">
-        <v>64007</v>
+      <c r="B24" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>134</v>
@@ -3394,8 +3397,8 @@
       <c r="O24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P24" s="11">
-        <v>64007</v>
+      <c r="P24" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q24" s="9" t="s">
         <v>27</v>
@@ -3406,8 +3409,8 @@
       <c r="S24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T24" s="11">
-        <v>64007</v>
+      <c r="T24" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U24" s="9"/>
       <c r="V24" s="12"/>
@@ -3435,8 +3438,8 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="7">
-        <v>64007</v>
+      <c r="B25" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>139</v>
@@ -3473,8 +3476,8 @@
       <c r="O25" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P25" s="11">
-        <v>64007</v>
+      <c r="P25" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q25" s="9" t="s">
         <v>27</v>
@@ -3485,8 +3488,8 @@
       <c r="S25" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T25" s="11">
-        <v>64007</v>
+      <c r="T25" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U25" s="9"/>
       <c r="V25" s="12"/>
@@ -3514,8 +3517,8 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="7">
-        <v>64007</v>
+      <c r="B26" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>139</v>
@@ -3552,8 +3555,8 @@
       <c r="O26" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P26" s="11">
-        <v>64007</v>
+      <c r="P26" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q26" s="9" t="s">
         <v>27</v>
@@ -3564,8 +3567,8 @@
       <c r="S26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T26" s="11">
-        <v>64007</v>
+      <c r="T26" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U26" s="9"/>
       <c r="V26" s="12"/>
@@ -3593,8 +3596,8 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="7">
-        <v>64007</v>
+      <c r="B27" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>144</v>
@@ -3631,8 +3634,8 @@
       <c r="O27" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P27" s="11">
-        <v>64007</v>
+      <c r="P27" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q27" s="9" t="s">
         <v>27</v>
@@ -3643,8 +3646,8 @@
       <c r="S27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T27" s="11">
-        <v>64007</v>
+      <c r="T27" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U27" s="9"/>
       <c r="V27" s="12"/>
@@ -3672,8 +3675,8 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="7">
-        <v>64007</v>
+      <c r="B28" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>144</v>
@@ -3710,8 +3713,8 @@
       <c r="O28" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P28" s="11">
-        <v>64007</v>
+      <c r="P28" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q28" s="9" t="s">
         <v>27</v>
@@ -3722,8 +3725,8 @@
       <c r="S28" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T28" s="11">
-        <v>64007</v>
+      <c r="T28" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U28" s="9"/>
       <c r="V28" s="12"/>
@@ -3751,8 +3754,8 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="7">
-        <v>64007</v>
+      <c r="B29" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>148</v>
@@ -3789,8 +3792,8 @@
       <c r="O29" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P29" s="11">
-        <v>64007</v>
+      <c r="P29" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q29" s="9" t="s">
         <v>27</v>
@@ -3801,8 +3804,8 @@
       <c r="S29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T29" s="11">
-        <v>64007</v>
+      <c r="T29" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U29" s="9"/>
       <c r="V29" s="12"/>
@@ -3830,8 +3833,8 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="7">
-        <v>64007</v>
+      <c r="B30" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>148</v>
@@ -3868,8 +3871,8 @@
       <c r="O30" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P30" s="11">
-        <v>64007</v>
+      <c r="P30" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q30" s="9" t="s">
         <v>27</v>
@@ -3880,8 +3883,8 @@
       <c r="S30" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T30" s="11">
-        <v>64007</v>
+      <c r="T30" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U30" s="9"/>
       <c r="V30" s="12"/>
@@ -3909,8 +3912,8 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="7">
-        <v>64007</v>
+      <c r="B31" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>152</v>
@@ -3947,8 +3950,8 @@
       <c r="O31" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P31" s="11">
-        <v>64007</v>
+      <c r="P31" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q31" s="9" t="s">
         <v>27</v>
@@ -3959,8 +3962,8 @@
       <c r="S31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T31" s="11">
-        <v>64007</v>
+      <c r="T31" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U31" s="9"/>
       <c r="V31" s="12"/>
@@ -3988,8 +3991,8 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="7">
-        <v>64007</v>
+      <c r="B32" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>152</v>
@@ -4026,8 +4029,8 @@
       <c r="O32" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P32" s="11">
-        <v>64007</v>
+      <c r="P32" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q32" s="9" t="s">
         <v>27</v>
@@ -4038,8 +4041,8 @@
       <c r="S32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T32" s="11">
-        <v>64007</v>
+      <c r="T32" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U32" s="9"/>
       <c r="V32" s="12"/>
@@ -4067,8 +4070,8 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="7">
-        <v>64007</v>
+      <c r="B33" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>156</v>
@@ -4105,8 +4108,8 @@
       <c r="O33" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P33" s="11">
-        <v>64007</v>
+      <c r="P33" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q33" s="9" t="s">
         <v>27</v>
@@ -4117,8 +4120,8 @@
       <c r="S33" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T33" s="11">
-        <v>64007</v>
+      <c r="T33" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U33" s="9"/>
       <c r="V33" s="12"/>
@@ -4146,8 +4149,8 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="7">
-        <v>64007</v>
+      <c r="B34" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>156</v>
@@ -4184,8 +4187,8 @@
       <c r="O34" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P34" s="11">
-        <v>64007</v>
+      <c r="P34" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q34" s="9" t="s">
         <v>27</v>
@@ -4196,8 +4199,8 @@
       <c r="S34" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T34" s="11">
-        <v>64007</v>
+      <c r="T34" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U34" s="9"/>
       <c r="V34" s="12"/>
@@ -4225,8 +4228,8 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="7">
-        <v>64007</v>
+      <c r="B35" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>160</v>
@@ -4263,8 +4266,8 @@
       <c r="O35" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P35" s="11">
-        <v>64007</v>
+      <c r="P35" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q35" s="9" t="s">
         <v>27</v>
@@ -4275,8 +4278,8 @@
       <c r="S35" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T35" s="11">
-        <v>64007</v>
+      <c r="T35" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U35" s="9"/>
       <c r="V35" s="12"/>
@@ -4304,8 +4307,8 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="7">
-        <v>64007</v>
+      <c r="B36" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>160</v>
@@ -4342,8 +4345,8 @@
       <c r="O36" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P36" s="11">
-        <v>64007</v>
+      <c r="P36" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q36" s="9" t="s">
         <v>27</v>
@@ -4354,8 +4357,8 @@
       <c r="S36" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T36" s="11">
-        <v>64007</v>
+      <c r="T36" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U36" s="9"/>
       <c r="V36" s="12"/>
@@ -4383,8 +4386,8 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="7">
-        <v>64007</v>
+      <c r="B37" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>165</v>
@@ -4421,8 +4424,8 @@
       <c r="O37" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P37" s="11">
-        <v>64007</v>
+      <c r="P37" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q37" s="9" t="s">
         <v>27</v>
@@ -4433,8 +4436,8 @@
       <c r="S37" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T37" s="11">
-        <v>64007</v>
+      <c r="T37" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U37" s="9"/>
       <c r="V37" s="12"/>
@@ -4462,8 +4465,8 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="7">
-        <v>64007</v>
+      <c r="B38" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>165</v>
@@ -4500,8 +4503,8 @@
       <c r="O38" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P38" s="11">
-        <v>64007</v>
+      <c r="P38" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q38" s="9" t="s">
         <v>27</v>
@@ -4512,8 +4515,8 @@
       <c r="S38" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T38" s="11">
-        <v>64007</v>
+      <c r="T38" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U38" s="9"/>
       <c r="V38" s="12"/>
@@ -4541,8 +4544,8 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="7">
-        <v>64007</v>
+      <c r="B39" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>169</v>
@@ -4579,8 +4582,8 @@
       <c r="O39" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P39" s="11">
-        <v>64007</v>
+      <c r="P39" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q39" s="9" t="s">
         <v>27</v>
@@ -4591,8 +4594,8 @@
       <c r="S39" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T39" s="11">
-        <v>64007</v>
+      <c r="T39" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U39" s="9"/>
       <c r="V39" s="12"/>
@@ -4620,8 +4623,8 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="7">
-        <v>64007</v>
+      <c r="B40" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>169</v>
@@ -4658,8 +4661,8 @@
       <c r="O40" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P40" s="11">
-        <v>64007</v>
+      <c r="P40" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q40" s="9" t="s">
         <v>27</v>
@@ -4670,8 +4673,8 @@
       <c r="S40" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T40" s="11">
-        <v>64007</v>
+      <c r="T40" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U40" s="9"/>
       <c r="V40" s="12"/>
@@ -4699,8 +4702,8 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B41" s="7">
-        <v>64007</v>
+      <c r="B41" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>173</v>
@@ -4737,8 +4740,8 @@
       <c r="O41" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P41" s="11">
-        <v>64007</v>
+      <c r="P41" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q41" s="9" t="s">
         <v>27</v>
@@ -4749,8 +4752,8 @@
       <c r="S41" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T41" s="11">
-        <v>64007</v>
+      <c r="T41" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U41" s="9"/>
       <c r="V41" s="12"/>
@@ -4778,8 +4781,8 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" s="7">
-        <v>64007</v>
+      <c r="B42" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>173</v>
@@ -4816,8 +4819,8 @@
       <c r="O42" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P42" s="11">
-        <v>64007</v>
+      <c r="P42" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q42" s="9" t="s">
         <v>27</v>
@@ -4828,8 +4831,8 @@
       <c r="S42" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T42" s="11">
-        <v>64007</v>
+      <c r="T42" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U42" s="9"/>
       <c r="V42" s="12"/>
@@ -4857,8 +4860,8 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B43" s="7">
-        <v>64007</v>
+      <c r="B43" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>178</v>
@@ -4895,8 +4898,8 @@
       <c r="O43" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P43" s="11">
-        <v>64007</v>
+      <c r="P43" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q43" s="9" t="s">
         <v>27</v>
@@ -4907,8 +4910,8 @@
       <c r="S43" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T43" s="11">
-        <v>64007</v>
+      <c r="T43" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U43" s="9"/>
       <c r="V43" s="12"/>
@@ -4936,8 +4939,8 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B44" s="7">
-        <v>64007</v>
+      <c r="B44" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>178</v>
@@ -4974,8 +4977,8 @@
       <c r="O44" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P44" s="11">
-        <v>64007</v>
+      <c r="P44" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q44" s="9" t="s">
         <v>27</v>
@@ -4986,8 +4989,8 @@
       <c r="S44" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T44" s="11">
-        <v>64007</v>
+      <c r="T44" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U44" s="9"/>
       <c r="V44" s="12"/>
@@ -5015,8 +5018,8 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B45" s="7">
-        <v>64007</v>
+      <c r="B45" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>182</v>
@@ -5053,8 +5056,8 @@
       <c r="O45" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P45" s="11">
-        <v>64007</v>
+      <c r="P45" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q45" s="9" t="s">
         <v>27</v>
@@ -5065,8 +5068,8 @@
       <c r="S45" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T45" s="11">
-        <v>64007</v>
+      <c r="T45" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U45" s="9"/>
       <c r="V45" s="12"/>
@@ -5094,8 +5097,8 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B46" s="7">
-        <v>64007</v>
+      <c r="B46" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>182</v>
@@ -5132,8 +5135,8 @@
       <c r="O46" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P46" s="11">
-        <v>64007</v>
+      <c r="P46" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q46" s="9" t="s">
         <v>27</v>
@@ -5144,8 +5147,8 @@
       <c r="S46" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T46" s="11">
-        <v>64007</v>
+      <c r="T46" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U46" s="9"/>
       <c r="V46" s="12"/>
@@ -5173,8 +5176,8 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B47" s="7">
-        <v>64007</v>
+      <c r="B47" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>186</v>
@@ -5211,8 +5214,8 @@
       <c r="O47" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P47" s="11">
-        <v>64007</v>
+      <c r="P47" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q47" s="9" t="s">
         <v>27</v>
@@ -5223,8 +5226,8 @@
       <c r="S47" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T47" s="11">
-        <v>64007</v>
+      <c r="T47" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U47" s="9"/>
       <c r="V47" s="12"/>
@@ -5252,8 +5255,8 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B48" s="7">
-        <v>64007</v>
+      <c r="B48" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>186</v>
@@ -5290,8 +5293,8 @@
       <c r="O48" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P48" s="11">
-        <v>64007</v>
+      <c r="P48" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q48" s="9" t="s">
         <v>27</v>
@@ -5302,8 +5305,8 @@
       <c r="S48" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T48" s="11">
-        <v>64007</v>
+      <c r="T48" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U48" s="9"/>
       <c r="V48" s="12"/>
@@ -5331,8 +5334,8 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B49" s="7">
-        <v>64007</v>
+      <c r="B49" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>191</v>
@@ -5369,8 +5372,8 @@
       <c r="O49" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P49" s="11">
-        <v>64007</v>
+      <c r="P49" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q49" s="9" t="s">
         <v>27</v>
@@ -5381,8 +5384,8 @@
       <c r="S49" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T49" s="11">
-        <v>64007</v>
+      <c r="T49" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U49" s="9"/>
       <c r="V49" s="12"/>
@@ -5410,8 +5413,8 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" s="7">
-        <v>64007</v>
+      <c r="B50" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>191</v>
@@ -5448,8 +5451,8 @@
       <c r="O50" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P50" s="11">
-        <v>64007</v>
+      <c r="P50" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q50" s="9" t="s">
         <v>27</v>
@@ -5460,8 +5463,8 @@
       <c r="S50" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T50" s="11">
-        <v>64007</v>
+      <c r="T50" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U50" s="9"/>
       <c r="V50" s="12"/>
@@ -5489,8 +5492,8 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="7">
-        <v>64007</v>
+      <c r="B51" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>195</v>
@@ -5527,8 +5530,8 @@
       <c r="O51" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P51" s="11">
-        <v>64007</v>
+      <c r="P51" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q51" s="9" t="s">
         <v>27</v>
@@ -5539,8 +5542,8 @@
       <c r="S51" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T51" s="11">
-        <v>64007</v>
+      <c r="T51" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U51" s="9"/>
       <c r="V51" s="12"/>
@@ -5568,8 +5571,8 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="7">
-        <v>64007</v>
+      <c r="B52" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>195</v>
@@ -5606,8 +5609,8 @@
       <c r="O52" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P52" s="11">
-        <v>64007</v>
+      <c r="P52" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q52" s="9" t="s">
         <v>27</v>
@@ -5618,8 +5621,8 @@
       <c r="S52" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T52" s="11">
-        <v>64007</v>
+      <c r="T52" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U52" s="9"/>
       <c r="V52" s="12"/>
@@ -5647,8 +5650,8 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B53" s="7">
-        <v>64007</v>
+      <c r="B53" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>200</v>
@@ -5685,8 +5688,8 @@
       <c r="O53" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P53" s="11">
-        <v>64007</v>
+      <c r="P53" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q53" s="9" t="s">
         <v>27</v>
@@ -5697,8 +5700,8 @@
       <c r="S53" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T53" s="11">
-        <v>64007</v>
+      <c r="T53" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U53" s="9"/>
       <c r="V53" s="12"/>
@@ -5726,8 +5729,8 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" s="7">
-        <v>64007</v>
+      <c r="B54" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>200</v>
@@ -5764,8 +5767,8 @@
       <c r="O54" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P54" s="11">
-        <v>64007</v>
+      <c r="P54" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q54" s="9" t="s">
         <v>27</v>
@@ -5776,8 +5779,8 @@
       <c r="S54" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T54" s="11">
-        <v>64007</v>
+      <c r="T54" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U54" s="9"/>
       <c r="V54" s="12"/>
@@ -5805,8 +5808,8 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B55" s="7">
-        <v>64007</v>
+      <c r="B55" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>204</v>
@@ -5843,8 +5846,8 @@
       <c r="O55" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P55" s="11">
-        <v>64007</v>
+      <c r="P55" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q55" s="9" t="s">
         <v>27</v>
@@ -5855,8 +5858,8 @@
       <c r="S55" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T55" s="11">
-        <v>64007</v>
+      <c r="T55" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U55" s="9"/>
       <c r="V55" s="12"/>
@@ -5884,8 +5887,8 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B56" s="7">
-        <v>64007</v>
+      <c r="B56" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>204</v>
@@ -5922,8 +5925,8 @@
       <c r="O56" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P56" s="11">
-        <v>64007</v>
+      <c r="P56" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q56" s="9" t="s">
         <v>27</v>
@@ -5934,8 +5937,8 @@
       <c r="S56" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T56" s="11">
-        <v>64007</v>
+      <c r="T56" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U56" s="9"/>
       <c r="V56" s="12"/>
@@ -5963,8 +5966,8 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B57" s="7">
-        <v>64007</v>
+      <c r="B57" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>208</v>
@@ -6001,8 +6004,8 @@
       <c r="O57" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P57" s="11">
-        <v>64007</v>
+      <c r="P57" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q57" s="9" t="s">
         <v>27</v>
@@ -6013,8 +6016,8 @@
       <c r="S57" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T57" s="11">
-        <v>64007</v>
+      <c r="T57" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U57" s="9"/>
       <c r="V57" s="12"/>
@@ -6042,8 +6045,8 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B58" s="7">
-        <v>64007</v>
+      <c r="B58" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>208</v>
@@ -6080,8 +6083,8 @@
       <c r="O58" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P58" s="11">
-        <v>64007</v>
+      <c r="P58" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q58" s="9" t="s">
         <v>27</v>
@@ -6092,8 +6095,8 @@
       <c r="S58" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T58" s="11">
-        <v>64007</v>
+      <c r="T58" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U58" s="9"/>
       <c r="V58" s="12"/>
@@ -6121,8 +6124,8 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B59" s="7">
-        <v>64007</v>
+      <c r="B59" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>212</v>
@@ -6159,8 +6162,8 @@
       <c r="O59" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P59" s="11">
-        <v>64007</v>
+      <c r="P59" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q59" s="9" t="s">
         <v>27</v>
@@ -6171,8 +6174,8 @@
       <c r="S59" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T59" s="11">
-        <v>64007</v>
+      <c r="T59" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U59" s="9"/>
       <c r="V59" s="12"/>
@@ -6200,8 +6203,8 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B60" s="7">
-        <v>64007</v>
+      <c r="B60" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>212</v>
@@ -6238,8 +6241,8 @@
       <c r="O60" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P60" s="11">
-        <v>64007</v>
+      <c r="P60" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q60" s="9" t="s">
         <v>27</v>
@@ -6250,8 +6253,8 @@
       <c r="S60" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T60" s="11">
-        <v>64007</v>
+      <c r="T60" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U60" s="9"/>
       <c r="V60" s="12"/>
@@ -6279,8 +6282,8 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B61" s="7">
-        <v>64007</v>
+      <c r="B61" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>216</v>
@@ -6317,8 +6320,8 @@
       <c r="O61" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P61" s="11">
-        <v>64007</v>
+      <c r="P61" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q61" s="9" t="s">
         <v>27</v>
@@ -6329,8 +6332,8 @@
       <c r="S61" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T61" s="11">
-        <v>64007</v>
+      <c r="T61" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U61" s="9"/>
       <c r="V61" s="12"/>
@@ -6358,8 +6361,8 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B62" s="7">
-        <v>64007</v>
+      <c r="B62" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>216</v>
@@ -6396,8 +6399,8 @@
       <c r="O62" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P62" s="11">
-        <v>64007</v>
+      <c r="P62" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q62" s="9" t="s">
         <v>27</v>
@@ -6408,8 +6411,8 @@
       <c r="S62" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T62" s="11">
-        <v>64007</v>
+      <c r="T62" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U62" s="9"/>
       <c r="V62" s="12"/>
@@ -6437,8 +6440,8 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B63" s="7">
-        <v>64007</v>
+      <c r="B63" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>220</v>
@@ -6475,8 +6478,8 @@
       <c r="O63" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P63" s="11">
-        <v>64007</v>
+      <c r="P63" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q63" s="9" t="s">
         <v>27</v>
@@ -6487,8 +6490,8 @@
       <c r="S63" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T63" s="11">
-        <v>64007</v>
+      <c r="T63" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U63" s="9"/>
       <c r="V63" s="12"/>
@@ -6516,8 +6519,8 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B64" s="7">
-        <v>64007</v>
+      <c r="B64" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>220</v>
@@ -6554,8 +6557,8 @@
       <c r="O64" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P64" s="11">
-        <v>64007</v>
+      <c r="P64" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q64" s="9" t="s">
         <v>27</v>
@@ -6566,8 +6569,8 @@
       <c r="S64" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T64" s="11">
-        <v>64007</v>
+      <c r="T64" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U64" s="9"/>
       <c r="V64" s="12"/>
@@ -6595,8 +6598,8 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B65" s="7">
-        <v>64007</v>
+      <c r="B65" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>224</v>
@@ -6633,8 +6636,8 @@
       <c r="O65" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P65" s="11">
-        <v>64007</v>
+      <c r="P65" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q65" s="9" t="s">
         <v>27</v>
@@ -6645,8 +6648,8 @@
       <c r="S65" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T65" s="11">
-        <v>64007</v>
+      <c r="T65" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U65" s="9"/>
       <c r="V65" s="12"/>
@@ -6674,8 +6677,8 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B66" s="7">
-        <v>64007</v>
+      <c r="B66" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>224</v>
@@ -6712,8 +6715,8 @@
       <c r="O66" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P66" s="11">
-        <v>64007</v>
+      <c r="P66" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q66" s="9" t="s">
         <v>27</v>
@@ -6724,8 +6727,8 @@
       <c r="S66" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T66" s="11">
-        <v>64007</v>
+      <c r="T66" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U66" s="9"/>
       <c r="V66" s="12"/>
@@ -6753,8 +6756,8 @@
         <f t="shared" ref="A67:A105" si="1" xml:space="preserve"> A66 + 1</f>
         <v>66</v>
       </c>
-      <c r="B67" s="7">
-        <v>64007</v>
+      <c r="B67" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>228</v>
@@ -6791,8 +6794,8 @@
       <c r="O67" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P67" s="11">
-        <v>64007</v>
+      <c r="P67" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q67" s="9" t="s">
         <v>27</v>
@@ -6803,8 +6806,8 @@
       <c r="S67" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T67" s="11">
-        <v>64007</v>
+      <c r="T67" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U67" s="9"/>
       <c r="V67" s="12"/>
@@ -6832,8 +6835,8 @@
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="B68" s="7">
-        <v>64007</v>
+      <c r="B68" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>228</v>
@@ -6870,8 +6873,8 @@
       <c r="O68" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P68" s="11">
-        <v>64007</v>
+      <c r="P68" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q68" s="9" t="s">
         <v>27</v>
@@ -6882,8 +6885,8 @@
       <c r="S68" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T68" s="11">
-        <v>64007</v>
+      <c r="T68" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U68" s="9"/>
       <c r="V68" s="12"/>
@@ -6911,8 +6914,8 @@
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B69" s="7">
-        <v>64007</v>
+      <c r="B69" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>232</v>
@@ -6949,8 +6952,8 @@
       <c r="O69" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P69" s="11">
-        <v>64007</v>
+      <c r="P69" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q69" s="9" t="s">
         <v>27</v>
@@ -6961,8 +6964,8 @@
       <c r="S69" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T69" s="11">
-        <v>64007</v>
+      <c r="T69" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U69" s="9"/>
       <c r="V69" s="12"/>
@@ -6990,8 +6993,8 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B70" s="7">
-        <v>64007</v>
+      <c r="B70" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>232</v>
@@ -7028,8 +7031,8 @@
       <c r="O70" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P70" s="11">
-        <v>64007</v>
+      <c r="P70" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q70" s="9" t="s">
         <v>27</v>
@@ -7040,8 +7043,8 @@
       <c r="S70" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T70" s="11">
-        <v>64007</v>
+      <c r="T70" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U70" s="9"/>
       <c r="V70" s="12"/>
@@ -7069,8 +7072,8 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B71" s="7">
-        <v>64007</v>
+      <c r="B71" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>236</v>
@@ -7107,8 +7110,8 @@
       <c r="O71" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P71" s="11">
-        <v>64007</v>
+      <c r="P71" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q71" s="9" t="s">
         <v>27</v>
@@ -7119,8 +7122,8 @@
       <c r="S71" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T71" s="11">
-        <v>64007</v>
+      <c r="T71" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U71" s="9"/>
       <c r="V71" s="12"/>
@@ -7148,8 +7151,8 @@
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B72" s="7">
-        <v>64007</v>
+      <c r="B72" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>236</v>
@@ -7186,8 +7189,8 @@
       <c r="O72" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P72" s="11">
-        <v>64007</v>
+      <c r="P72" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q72" s="9" t="s">
         <v>27</v>
@@ -7198,8 +7201,8 @@
       <c r="S72" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T72" s="11">
-        <v>64007</v>
+      <c r="T72" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U72" s="9"/>
       <c r="V72" s="12"/>
@@ -7227,8 +7230,8 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B73" s="7">
-        <v>64007</v>
+      <c r="B73" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>240</v>
@@ -7265,8 +7268,8 @@
       <c r="O73" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P73" s="11">
-        <v>64007</v>
+      <c r="P73" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q73" s="9" t="s">
         <v>27</v>
@@ -7277,8 +7280,8 @@
       <c r="S73" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T73" s="11">
-        <v>64007</v>
+      <c r="T73" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U73" s="9"/>
       <c r="V73" s="12"/>
@@ -7306,8 +7309,8 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B74" s="7">
-        <v>64007</v>
+      <c r="B74" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>240</v>
@@ -7344,8 +7347,8 @@
       <c r="O74" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P74" s="11">
-        <v>64007</v>
+      <c r="P74" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q74" s="9" t="s">
         <v>27</v>
@@ -7356,8 +7359,8 @@
       <c r="S74" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T74" s="11">
-        <v>64007</v>
+      <c r="T74" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U74" s="9"/>
       <c r="V74" s="12"/>
@@ -7385,8 +7388,8 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B75" s="7">
-        <v>64007</v>
+      <c r="B75" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>244</v>
@@ -7423,8 +7426,8 @@
       <c r="O75" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P75" s="11">
-        <v>64007</v>
+      <c r="P75" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q75" s="9" t="s">
         <v>27</v>
@@ -7435,8 +7438,8 @@
       <c r="S75" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T75" s="11">
-        <v>64007</v>
+      <c r="T75" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U75" s="9"/>
       <c r="V75" s="12"/>
@@ -7464,8 +7467,8 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B76" s="7">
-        <v>64007</v>
+      <c r="B76" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>244</v>
@@ -7502,8 +7505,8 @@
       <c r="O76" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P76" s="11">
-        <v>64007</v>
+      <c r="P76" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q76" s="9" t="s">
         <v>27</v>
@@ -7514,8 +7517,8 @@
       <c r="S76" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T76" s="11">
-        <v>64007</v>
+      <c r="T76" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U76" s="9"/>
       <c r="V76" s="12"/>
@@ -7543,8 +7546,8 @@
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B77" s="7">
-        <v>64007</v>
+      <c r="B77" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>248</v>
@@ -7581,8 +7584,8 @@
       <c r="O77" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P77" s="11">
-        <v>64007</v>
+      <c r="P77" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q77" s="9" t="s">
         <v>27</v>
@@ -7593,8 +7596,8 @@
       <c r="S77" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T77" s="11">
-        <v>64007</v>
+      <c r="T77" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U77" s="9"/>
       <c r="V77" s="12"/>
@@ -7622,8 +7625,8 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="B78" s="7">
-        <v>64007</v>
+      <c r="B78" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>248</v>
@@ -7660,8 +7663,8 @@
       <c r="O78" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P78" s="11">
-        <v>64007</v>
+      <c r="P78" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q78" s="9" t="s">
         <v>27</v>
@@ -7672,8 +7675,8 @@
       <c r="S78" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T78" s="11">
-        <v>64007</v>
+      <c r="T78" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U78" s="9"/>
       <c r="V78" s="12"/>
@@ -7701,8 +7704,8 @@
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="B79" s="7">
-        <v>64007</v>
+      <c r="B79" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>252</v>
@@ -7739,8 +7742,8 @@
       <c r="O79" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P79" s="11">
-        <v>64007</v>
+      <c r="P79" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q79" s="9" t="s">
         <v>27</v>
@@ -7751,8 +7754,8 @@
       <c r="S79" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T79" s="11">
-        <v>64007</v>
+      <c r="T79" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U79" s="9"/>
       <c r="V79" s="12"/>
@@ -7780,8 +7783,8 @@
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="B80" s="7">
-        <v>64007</v>
+      <c r="B80" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>252</v>
@@ -7818,8 +7821,8 @@
       <c r="O80" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P80" s="11">
-        <v>64007</v>
+      <c r="P80" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q80" s="9" t="s">
         <v>27</v>
@@ -7830,8 +7833,8 @@
       <c r="S80" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T80" s="11">
-        <v>64007</v>
+      <c r="T80" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U80" s="9"/>
       <c r="V80" s="12"/>
@@ -7859,8 +7862,8 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B81" s="7">
-        <v>64007</v>
+      <c r="B81" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>256</v>
@@ -7899,8 +7902,8 @@
       <c r="O81" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P81" s="11">
-        <v>64007</v>
+      <c r="P81" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q81" s="9" t="s">
         <v>27</v>
@@ -7911,8 +7914,8 @@
       <c r="S81" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T81" s="11">
-        <v>64007</v>
+      <c r="T81" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U81" s="9"/>
       <c r="V81" s="12"/>
@@ -7940,8 +7943,8 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B82" s="7">
-        <v>64007</v>
+      <c r="B82" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>256</v>
@@ -7980,8 +7983,8 @@
       <c r="O82" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P82" s="11">
-        <v>64007</v>
+      <c r="P82" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q82" s="9" t="s">
         <v>27</v>
@@ -7992,8 +7995,8 @@
       <c r="S82" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T82" s="11">
-        <v>64007</v>
+      <c r="T82" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U82" s="9"/>
       <c r="V82" s="12"/>
@@ -8021,8 +8024,8 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B83" s="7">
-        <v>64007</v>
+      <c r="B83" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>261</v>
@@ -8061,8 +8064,8 @@
       <c r="O83" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P83" s="11">
-        <v>64007</v>
+      <c r="P83" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q83" s="9" t="s">
         <v>27</v>
@@ -8073,8 +8076,8 @@
       <c r="S83" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T83" s="11">
-        <v>64007</v>
+      <c r="T83" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U83" s="9"/>
       <c r="V83" s="12"/>
@@ -8102,8 +8105,8 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="B84" s="7">
-        <v>64007</v>
+      <c r="B84" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>261</v>
@@ -8142,8 +8145,8 @@
       <c r="O84" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P84" s="11">
-        <v>64007</v>
+      <c r="P84" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q84" s="9" t="s">
         <v>27</v>
@@ -8154,8 +8157,8 @@
       <c r="S84" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T84" s="11">
-        <v>64007</v>
+      <c r="T84" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U84" s="9"/>
       <c r="V84" s="12"/>
@@ -8183,8 +8186,8 @@
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="B85" s="7">
-        <v>64007</v>
+      <c r="B85" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>266</v>
@@ -8223,8 +8226,8 @@
       <c r="O85" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P85" s="11">
-        <v>64007</v>
+      <c r="P85" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q85" s="9" t="s">
         <v>27</v>
@@ -8235,8 +8238,8 @@
       <c r="S85" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T85" s="11">
-        <v>64007</v>
+      <c r="T85" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U85" s="9"/>
       <c r="V85" s="12"/>
@@ -8264,8 +8267,8 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B86" s="7">
-        <v>64007</v>
+      <c r="B86" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>266</v>
@@ -8304,8 +8307,8 @@
       <c r="O86" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P86" s="11">
-        <v>64007</v>
+      <c r="P86" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q86" s="9" t="s">
         <v>27</v>
@@ -8316,8 +8319,8 @@
       <c r="S86" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T86" s="11">
-        <v>64007</v>
+      <c r="T86" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U86" s="9"/>
       <c r="V86" s="12"/>
@@ -8345,8 +8348,8 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B87" s="7">
-        <v>64007</v>
+      <c r="B87" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>271</v>
@@ -8385,8 +8388,8 @@
       <c r="O87" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P87" s="11">
-        <v>64007</v>
+      <c r="P87" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q87" s="9" t="s">
         <v>27</v>
@@ -8397,8 +8400,8 @@
       <c r="S87" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T87" s="11">
-        <v>64007</v>
+      <c r="T87" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U87" s="9"/>
       <c r="V87" s="12"/>
@@ -8426,8 +8429,8 @@
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="B88" s="7">
-        <v>64007</v>
+      <c r="B88" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>271</v>
@@ -8466,8 +8469,8 @@
       <c r="O88" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P88" s="11">
-        <v>64007</v>
+      <c r="P88" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q88" s="9" t="s">
         <v>27</v>
@@ -8478,8 +8481,8 @@
       <c r="S88" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T88" s="11">
-        <v>64007</v>
+      <c r="T88" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U88" s="9"/>
       <c r="V88" s="12"/>
@@ -8507,8 +8510,8 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="B89" s="7">
-        <v>64007</v>
+      <c r="B89" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>276</v>
@@ -8545,8 +8548,8 @@
       <c r="O89" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P89" s="11">
-        <v>64007</v>
+      <c r="P89" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q89" s="9" t="s">
         <v>27</v>
@@ -8557,8 +8560,8 @@
       <c r="S89" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T89" s="11">
-        <v>64007</v>
+      <c r="T89" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U89" s="9"/>
       <c r="V89" s="12"/>
@@ -8586,8 +8589,8 @@
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="B90" s="7">
-        <v>64007</v>
+      <c r="B90" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>276</v>
@@ -8624,8 +8627,8 @@
       <c r="O90" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P90" s="11">
-        <v>64007</v>
+      <c r="P90" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q90" s="9" t="s">
         <v>27</v>
@@ -8636,8 +8639,8 @@
       <c r="S90" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T90" s="11">
-        <v>64007</v>
+      <c r="T90" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U90" s="9"/>
       <c r="V90" s="12"/>
@@ -8665,8 +8668,8 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B91" s="7">
-        <v>64007</v>
+      <c r="B91" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>280</v>
@@ -8703,8 +8706,8 @@
       <c r="O91" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P91" s="11">
-        <v>64007</v>
+      <c r="P91" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q91" s="9" t="s">
         <v>27</v>
@@ -8715,8 +8718,8 @@
       <c r="S91" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T91" s="11">
-        <v>64007</v>
+      <c r="T91" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U91" s="9"/>
       <c r="V91" s="12"/>
@@ -8744,8 +8747,8 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="B92" s="7">
-        <v>64007</v>
+      <c r="B92" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>280</v>
@@ -8782,8 +8785,8 @@
       <c r="O92" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="P92" s="11">
-        <v>64007</v>
+      <c r="P92" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q92" s="9" t="s">
         <v>27</v>
@@ -8794,8 +8797,8 @@
       <c r="S92" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T92" s="11">
-        <v>64007</v>
+      <c r="T92" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U92" s="9"/>
       <c r="V92" s="12"/>
@@ -8823,8 +8826,8 @@
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="B93" s="7">
-        <v>64007</v>
+      <c r="B93" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>284</v>
@@ -8861,8 +8864,8 @@
       <c r="O93" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="P93" s="11">
-        <v>64007</v>
+      <c r="P93" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q93" s="9" t="s">
         <v>36</v>
@@ -8873,8 +8876,8 @@
       <c r="S93" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T93" s="11">
-        <v>64007</v>
+      <c r="T93" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U93" s="9"/>
       <c r="V93" s="12"/>
@@ -8902,8 +8905,8 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B94" s="7">
-        <v>64007</v>
+      <c r="B94" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>284</v>
@@ -8940,8 +8943,8 @@
       <c r="O94" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="P94" s="11">
-        <v>64007</v>
+      <c r="P94" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q94" s="9" t="s">
         <v>36</v>
@@ -8952,8 +8955,8 @@
       <c r="S94" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T94" s="11">
-        <v>64007</v>
+      <c r="T94" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U94" s="9"/>
       <c r="V94" s="12"/>
@@ -8981,8 +8984,8 @@
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B95" s="7">
-        <v>64007</v>
+      <c r="B95" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>290</v>
@@ -9021,8 +9024,8 @@
       <c r="O95" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P95" s="11">
-        <v>64007</v>
+      <c r="P95" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q95" s="9" t="s">
         <v>27</v>
@@ -9033,8 +9036,8 @@
       <c r="S95" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="T95" s="11">
-        <v>64007</v>
+      <c r="T95" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U95" s="9"/>
       <c r="V95" s="12"/>
@@ -9062,8 +9065,8 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="B96" s="7">
-        <v>64007</v>
+      <c r="B96" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>296</v>
@@ -9102,8 +9105,8 @@
       <c r="O96" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P96" s="11">
-        <v>64007</v>
+      <c r="P96" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q96" s="9" t="s">
         <v>27</v>
@@ -9114,8 +9117,8 @@
       <c r="S96" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="T96" s="11">
-        <v>64007</v>
+      <c r="T96" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U96" s="9"/>
       <c r="V96" s="12"/>
@@ -9143,8 +9146,8 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="B97" s="7">
-        <v>64007</v>
+      <c r="B97" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>300</v>
@@ -9181,8 +9184,8 @@
       <c r="O97" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P97" s="11">
-        <v>64007</v>
+      <c r="P97" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q97" s="9" t="s">
         <v>36</v>
@@ -9193,8 +9196,8 @@
       <c r="S97" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="T97" s="11">
-        <v>64007</v>
+      <c r="T97" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U97" s="9"/>
       <c r="V97" s="12"/>
@@ -9222,8 +9225,8 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="B98" s="7">
-        <v>64007</v>
+      <c r="B98" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>307</v>
@@ -9260,8 +9263,8 @@
       <c r="O98" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P98" s="11">
-        <v>64007</v>
+      <c r="P98" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q98" s="9" t="s">
         <v>36</v>
@@ -9272,8 +9275,8 @@
       <c r="S98" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="T98" s="11">
-        <v>64007</v>
+      <c r="T98" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U98" s="9"/>
       <c r="V98" s="12"/>
@@ -9301,8 +9304,8 @@
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="B99" s="7">
-        <v>64007</v>
+      <c r="B99" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>313</v>
@@ -9339,8 +9342,8 @@
       <c r="O99" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="P99" s="11">
-        <v>64007</v>
+      <c r="P99" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q99" s="9" t="s">
         <v>36</v>
@@ -9351,8 +9354,8 @@
       <c r="S99" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="T99" s="11">
-        <v>64007</v>
+      <c r="T99" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="U99" s="9"/>
       <c r="V99" s="12"/>
@@ -9380,8 +9383,8 @@
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B100" s="7">
-        <v>64007</v>
+      <c r="B100" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>320</v>
@@ -9418,8 +9421,8 @@
       <c r="O100" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="P100" s="11">
-        <v>64007</v>
+      <c r="P100" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q100" s="9"/>
       <c r="R100" s="10"/>
@@ -9451,8 +9454,8 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B101" s="7">
-        <v>64007</v>
+      <c r="B101" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>324</v>
@@ -9489,8 +9492,8 @@
       <c r="O101" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="P101" s="11">
-        <v>64007</v>
+      <c r="P101" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q101" s="9"/>
       <c r="R101" s="10"/>
@@ -9522,8 +9525,8 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="B102" s="7">
-        <v>64007</v>
+      <c r="B102" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>329</v>
@@ -9562,8 +9565,8 @@
       <c r="O102" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="P102" s="11">
-        <v>64007</v>
+      <c r="P102" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q102" s="9"/>
       <c r="R102" s="10"/>
@@ -9595,8 +9598,8 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="B103" s="7">
-        <v>64007</v>
+      <c r="B103" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>334</v>
@@ -9635,8 +9638,8 @@
       <c r="O103" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="P103" s="11">
-        <v>64007</v>
+      <c r="P103" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q103" s="9"/>
       <c r="R103" s="10"/>
@@ -9668,8 +9671,8 @@
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="B104" s="7">
-        <v>64007</v>
+      <c r="B104" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>339</v>
@@ -9706,8 +9709,8 @@
       <c r="O104" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="P104" s="11">
-        <v>64007</v>
+      <c r="P104" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q104" s="9"/>
       <c r="R104" s="10"/>
@@ -9739,8 +9742,8 @@
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B105" s="7">
-        <v>64007</v>
+      <c r="B105" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>343</v>
@@ -9779,8 +9782,8 @@
       <c r="O105" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="P105" s="11">
-        <v>64007</v>
+      <c r="P105" s="11" t="s">
+        <v>348</v>
       </c>
       <c r="Q105" s="9"/>
       <c r="R105" s="10"/>
@@ -9808,6 +9811,7 @@
       <c r="AN105" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AN1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>